<commit_message>
[ANV] almost finished with Th232 notebook
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A4C905-A04F-5C40-8117-793FECC749D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC47FCA9-5F69-E248-85AA-32957734FFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Decay</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Lambda1</t>
+  </si>
+  <si>
+    <t>branching ratio alpha (%)</t>
+  </si>
+  <si>
+    <t>branching ratio beta (%)</t>
   </si>
 </sst>
 </file>
@@ -72,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,10 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E56D091-102E-4A44-B40D-B7C123D87265}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,6 +758,28 @@
         <v>2425430924282841</v>
       </c>
     </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>64.06</v>
+      </c>
+      <c r="C17">
+        <v>35.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ANV] get some more data in the spreadsheet
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC47FCA9-5F69-E248-85AA-32957734FFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4A9972-2A52-2742-B9D1-FCD69ACB09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
+    <sheet name="U235" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Decay</t>
   </si>
@@ -125,11 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E56D091-102E-4A44-B40D-B7C123D87265}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,4 +785,527 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1176D-7192-D146-B909-C00911AAFABB}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>704000000</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/LN(2)</f>
+        <v>1015657308.7858303</v>
+      </c>
+      <c r="D2" s="2">
+        <f>1/C2</f>
+        <v>9.8458406329537694E-10</v>
+      </c>
+      <c r="E2" s="2">
+        <f>1/F2</f>
+        <v>1.0004224491540428</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2/$G$2</f>
+        <v>0.99957772923388521</v>
+      </c>
+      <c r="G2" s="2">
+        <v>9.8500000000000001E-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>25.52/24/365</f>
+        <v>2.91324200913242E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C17" si="0">B3/LN(2)</f>
+        <v>4.2029197994847426E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D17" si="1">1/C3</f>
+        <v>237.9298315715173</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E17" si="2">1/F3</f>
+        <v>4.1398760024924713E-12</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F17" si="3">D3/$G$2</f>
+        <v>241553128499.00232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>32760</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>47262.689539522442</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1158338844931175E-5</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="2"/>
+        <v>4.6553749196429605E-5</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="3"/>
+        <v>21480.547050691548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>21.771999999999998</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>31.410356430234511</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1836633316183416E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0939201083780993E-8</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="3"/>
+        <v>32321455.143333416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>18.697/365</f>
+        <v>5.122465753424657E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>7.3901559395893004E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>13.531514195024874</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="2"/>
+        <v>7.2793036004954601E-11</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>13737577862.969416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>22/60/24/365</f>
+        <v>4.185692541856925E-5</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0386778728229057E-5</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>16559.916277377604</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="2"/>
+        <v>5.9480977047305625E-14</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>16812097743530.562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>11.43/365</f>
+        <v>3.1315068493150681E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5178094020166711E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>22.134621251476823</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="2"/>
+        <v>4.4500422609864206E-11</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>22471696702.006927</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>56/60/60/24/365</f>
+        <v>1.7757483510908167E-6</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5618633399854751E-6</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>390340.88368104352</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5234353898856928E-15</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>396285161097506.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>3.96/60/60/24/365</f>
+        <v>1.2557077625570777E-7</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8116033618468721E-7</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>5519972.0924592</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.784429311419169E-16</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>5604032581176853</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>7.6/60/24/365</f>
+        <v>1.445966514459665E-5</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0860887197024583E-5</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>47936.599750303591</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0547973889069215E-14</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>48666598731272.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>0.000001781/60/60/24/365</f>
+        <v>5.6475139523084737E-14</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8.1476403723466653E-14</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>12273492131464.588</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="2"/>
+        <v>8.0254257667614652E-23</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2460398103009734E+22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>0.0000001/60/60/24/365</f>
+        <v>3.1709791983764578E-15</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>4.5747559642597765E-15</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>218590894861384.41</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="2"/>
+        <v>4.50613462479588E-24</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2191969021460346E+23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>36.1/60/24/365</f>
+        <v>6.8683409436834093E-5</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9089214185866782E-5</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>10091.915736906018</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="2"/>
+        <v>9.7602875973078785E-14</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="3"/>
+        <v>10245599732899.51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>2.14/60/24/365</f>
+        <v>4.071537290715373E-6</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>5.8739866581095541E-6</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>170242.12995434919</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="2"/>
+        <v>5.7858768582379102E-15</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="3"/>
+        <v>172834649699846.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <f>0.516/60/60/24/365</f>
+        <v>1.6362252663622526E-8</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.360574077558045E-8</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>42362576.523524098</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3251654663946746E-17</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="3"/>
+        <v>4.300769190205492E+16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f>4.77/60/24/365</f>
+        <v>9.0753424657534235E-6</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3092951569711481E-5</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>76376.972348492098</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.289655729616581E-14</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>77540073450245.781</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <f>0.9862*100</f>
+        <v>98.61999999999999</v>
+      </c>
+      <c r="C25">
+        <f>0.0138*100</f>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <f>0.9999*100</f>
+        <v>99.99</v>
+      </c>
+      <c r="C26" s="2">
+        <f>0.006*100</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <f>0.936*100</f>
+        <v>93.600000000000009</v>
+      </c>
+      <c r="C27">
+        <f>0.064*100</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <f>1*100</f>
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <f>0.00023*100</f>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <f>0.9972*100</f>
+        <v>99.72</v>
+      </c>
+      <c r="C29">
+        <f>0.0028*100</f>
+        <v>0.27999999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] added info for U238 decay chain
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4A9972-2A52-2742-B9D1-FCD69ACB09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F7132B-F078-6B47-B2AA-08553AC50897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
     <sheet name="U235" sheetId="2" r:id="rId2"/>
+    <sheet name="U238" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>Decay</t>
   </si>
@@ -126,12 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1176D-7192-D146-B909-C00911AAFABB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1179,11 +1179,11 @@
         <v>172834649699846.91</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <f>0.516/60/60/24/365</f>
         <v>1.6362252663622526E-8</v>
       </c>
@@ -1303,6 +1303,564 @@
       <c r="C29">
         <f>0.0028*100</f>
         <v>0.27999999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA6BC9F-6F57-874B-973E-14E935690D92}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4468000000</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/LN(2)</f>
+        <v>6445961442.6918888</v>
+      </c>
+      <c r="D2" s="2">
+        <f>1/C2</f>
+        <v>1.5513589538047119E-10</v>
+      </c>
+      <c r="E2" s="2">
+        <f>1/F2</f>
+        <v>0.99912402361724273</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2/$G$2</f>
+        <v>1.0008767443901367</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.5500000000000001E-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>24.1/365</f>
+        <v>6.6027397260273971E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C19" si="0">B3/LN(2)</f>
+        <v>9.5257398590202796E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D19" si="1">1/C3</f>
+        <v>10.497872236696267</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E19" si="2">1/F3</f>
+        <v>1.4764896781481431E-11</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F19" si="3">D3/$G$2</f>
+        <v>67728207978.685593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <f>1.159/60/24/365</f>
+        <v>2.2050989345509894E-6</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1812852975462493E-6</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>314338.35901838419</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="2"/>
+        <v>4.9309922111966865E-16</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="3"/>
+        <v>2027989413021833.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>245500</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>354181.63253824052</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>2.82341010411383E-6</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="2"/>
+        <v>5.4898153043427292E-5</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="3"/>
+        <v>18215.549058798901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>75400</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>108779.20608302785</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>9.1929334291769932E-6</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6860776942869315E-5</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>59309.247930174148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1600</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>2308.3120654223417</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>4.3321698784996578E-4</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="2"/>
+        <v>3.5778837014046299E-7</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>2794948.3087094566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>3.8235/365</f>
+        <v>1.0475342465753426E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5112724626956033E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>66.169405231955025</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3424723171781853E-12</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>426899388593.25818</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>3.098/60/24/365</f>
+        <v>5.8942161339421609E-6</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5035563863660734E-6</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>117597.85606917601</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3180512398867414E-15</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>758695845607587.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>1.5/60/60/24/365</f>
+        <v>4.7564687975646879E-8</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8621339463896667E-8</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>14572726.324092289</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0636307616903983E-17</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>9.4017589187692192E+16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>27.06/60/24/365</f>
+        <v>5.1484018264840178E-5</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4275737835721736E-5</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>13463.346566973662</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="2"/>
+        <v>1.151273936453687E-14</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>86860300432088.141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>19.9/60/24/365</f>
+        <v>3.7861491628614916E-5</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>5.4622586213261743E-5</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>18307.445130769207</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="2"/>
+        <v>8.4665008630555703E-15</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="3"/>
+        <v>118112549230769.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>0.0001636/60/60/24/365</f>
+        <v>5.1877219685438864E-12</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4843007575289955E-12</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>133613016418.9391</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1600666174169944E-21</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="3"/>
+        <v>8.6201946076734895E+20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>1.3/60/24/365</f>
+        <v>2.4733637747336381E-6</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5683096521226271E-6</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>280244.73700177477</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="2"/>
+        <v>5.5308799607900715E-16</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="3"/>
+        <v>1808030561301772.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>22.2</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>32.02782990773499</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1222845971168707E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="2"/>
+        <v>4.9643136356989229E-9</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="3"/>
+        <v>201437715.94302392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f>5.012/365</f>
+        <v>1.3731506849315067E-2</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9810376835439684E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>50.478595551552282</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0706084094931515E-12</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="3"/>
+        <v>325668358397.11145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f>138.376/365</f>
+        <v>0.37911232876712331</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54694347665219512</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8283424936721686</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="2"/>
+        <v>8.4776238881090251E-11</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="3"/>
+        <v>11795758023.69141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f>8.32/60/24/365</f>
+        <v>1.582952815829528E-5</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>2.283718177358481E-5</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>43788.24015652731</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="2"/>
+        <v>3.5397631749056459E-15</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="3"/>
+        <v>282504775203402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f>4.202/60/24/365</f>
+        <v>7.9946727549467287E-6</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1533874737091752E-5</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>86701.132342291108</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7877505842492216E-15</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="3"/>
+        <v>559362144143813.56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <f>0.0002*100</f>
+        <v>0.02</v>
+      </c>
+      <c r="C25">
+        <f>0.9998*100</f>
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f>0.9998*100</f>
+        <v>99.98</v>
+      </c>
+      <c r="C26" s="2">
+        <f>0.0002*100</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <f>1*100</f>
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <f>0.000000019*100</f>
+        <v>1.9000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <f>1*100</f>
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <f>0.0000013*100</f>
+        <v>1.3000000000000002E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ANV] updated decay chain data
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F7132B-F078-6B47-B2AA-08553AC50897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B9AD2-A871-0C46-8E05-3EB3FB6BCF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
     <sheet name="U235" sheetId="2" r:id="rId2"/>
     <sheet name="U238" sheetId="3" r:id="rId3"/>
+    <sheet name="SE Results" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Decay</t>
   </si>
@@ -66,11 +67,47 @@
   <si>
     <t>branching ratio beta (%)</t>
   </si>
+  <si>
+    <t>isotopes</t>
+  </si>
+  <si>
+    <t>overall contamination (ppm)</t>
+  </si>
+  <si>
+    <t>902320-Th</t>
+  </si>
+  <si>
+    <t>902280-Th</t>
+  </si>
+  <si>
+    <t>882240-Ra</t>
+  </si>
+  <si>
+    <t>232-Th (for 3e-14 ppm)</t>
+  </si>
+  <si>
+    <t>scaled</t>
+  </si>
+  <si>
+    <t>862200-Rn</t>
+  </si>
+  <si>
+    <t>842160-Po</t>
+  </si>
+  <si>
+    <t>842120-Po</t>
+  </si>
+  <si>
+    <t>832120-Bi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -80,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +133,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,11 +170,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA6BC9F-6F57-874B-973E-14E935690D92}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,4 +1912,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2*($D$2/0.00000000000003)</f>
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.9999999999999998E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
+        <f>4.07056E-24</f>
+        <v>4.0705599999999999E-24</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C8" si="0">B3*($D$2/0.00000000000003)</f>
+        <v>4.0705599999999999E-24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6">
+        <f>2.11268E-26</f>
+        <v>2.1126800000000001E-26</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1126800000000001E-26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.7546900000000003E-30</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7546900000000003E-30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6">
+        <v>9.8039200000000002E-33</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8039200000000002E-33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.2898000000000001E-38</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2898000000000001E-38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
+        <f>2.45902E-28</f>
+        <v>2.4590199999999999E-28</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4590199999999999E-28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] found mistake in U235 decay chain
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324B9AD2-A871-0C46-8E05-3EB3FB6BCF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC18AD34-FF14-DC42-801F-528DE575947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="13140" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1176D-7192-D146-B909-C00911AAFABB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,24 +1130,24 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f>0.000001781/60/60/24/365</f>
-        <v>5.6475139523084737E-14</v>
+        <f>0.001781/60/60/24/365</f>
+        <v>5.6475139523084721E-11</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>8.1476403723466653E-14</v>
+        <v>8.1476403723466624E-11</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>12273492131464.588</v>
+        <v>12273492131.464592</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>8.0254257667614652E-23</v>
+        <v>8.0254257667614621E-20</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="3"/>
-        <v>1.2460398103009734E+22</v>
+        <v>1.2460398103009739E+19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1155,24 +1155,24 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f>0.0000001/60/60/24/365</f>
-        <v>3.1709791983764578E-15</v>
+        <f>0.0001/60/60/24/365</f>
+        <v>3.1709791983764588E-12</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>4.5747559642597765E-15</v>
+        <v>4.5747559642597778E-12</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>218590894861384.41</v>
+        <v>218590894861.38434</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>4.50613462479588E-24</v>
+        <v>4.5061346247958812E-21</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="3"/>
-        <v>2.2191969021460346E+23</v>
+        <v>2.2191969021460339E+20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA6BC9F-6F57-874B-973E-14E935690D92}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="117" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1918,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[ANV] updated the decay chain results
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC18AD34-FF14-DC42-801F-528DE575947C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4FBAAD-3536-074A-AE55-1E934CAF37AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Decay</t>
   </si>
@@ -99,6 +99,84 @@
   </si>
   <si>
     <t>832120-Bi</t>
+  </si>
+  <si>
+    <t>238-U (for 9e-15 ppm)</t>
+  </si>
+  <si>
+    <t>922380-U</t>
+  </si>
+  <si>
+    <t>922340-U</t>
+  </si>
+  <si>
+    <t>902300-Th</t>
+  </si>
+  <si>
+    <t>882260-Ra</t>
+  </si>
+  <si>
+    <t>862220-Rn</t>
+  </si>
+  <si>
+    <t>842180-Po</t>
+  </si>
+  <si>
+    <t>852180-At</t>
+  </si>
+  <si>
+    <t>832140-Bi</t>
+  </si>
+  <si>
+    <t>842140-Po</t>
+  </si>
+  <si>
+    <t>822100-Pb</t>
+  </si>
+  <si>
+    <t>832100-Bi</t>
+  </si>
+  <si>
+    <t>842100-Po</t>
+  </si>
+  <si>
+    <t>235-U (for 6.4836e-17 ppm)</t>
+  </si>
+  <si>
+    <t>922350-U</t>
+  </si>
+  <si>
+    <t>912310-Pa</t>
+  </si>
+  <si>
+    <t>892270-Ac</t>
+  </si>
+  <si>
+    <t>902270-Th</t>
+  </si>
+  <si>
+    <t>872230-Fr</t>
+  </si>
+  <si>
+    <t>882230-Ra</t>
+  </si>
+  <si>
+    <t>852190-At</t>
+  </si>
+  <si>
+    <t>862190-Rn</t>
+  </si>
+  <si>
+    <t>842150-Po</t>
+  </si>
+  <si>
+    <t>852150-At</t>
+  </si>
+  <si>
+    <t>832110-Bi</t>
+  </si>
+  <si>
+    <t>842110-Po</t>
   </si>
 </sst>
 </file>
@@ -837,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1176D-7192-D146-B909-C00911AAFABB}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA6BC9F-6F57-874B-973E-14E935690D92}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1916,16 +1994,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
   </cols>
@@ -2034,6 +2112,332 @@
         <v>2.4590199999999999E-28</v>
       </c>
     </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8.9999999999999995E-15</v>
+      </c>
+      <c r="C11" s="6">
+        <f>B11/($D$11/0.000000000000009)</f>
+        <v>8.9999999999999995E-15</v>
+      </c>
+      <c r="D11" s="2">
+        <v>8.9999999999999995E-15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6">
+        <f>4.94533E-19</f>
+        <v>4.9453300000000002E-19</v>
+      </c>
+      <c r="C12" s="6">
+        <f>B12/($D$11/0.000000000000009)</f>
+        <v>4.9453300000000002E-19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6">
+        <f>1.51782E-19</f>
+        <v>1.5178200000000001E-19</v>
+      </c>
+      <c r="C13" s="6">
+        <f>B13/($D$11/0.000000000000009)</f>
+        <v>1.5178200000000001E-19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6">
+        <f>3.22604E-21</f>
+        <v>3.22604E-21</v>
+      </c>
+      <c r="C14" s="6">
+        <f>B14/($D$11/0.000000000000009)</f>
+        <v>3.22604E-21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2.1078800000000001E-26</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:C22" si="1">B15/($D$11/0.000000000000009)</f>
+        <v>2.1078800000000001E-26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1.9150299999999999E-35</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9150299999999999E-35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.1858500000000001E-29</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>1.1858500000000001E-29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.04395E-35</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="1"/>
+        <v>1.04395E-35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.62767E-25</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="1"/>
+        <v>7.62767E-25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7.6275999999999997E-29</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6275999999999997E-29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.7609400000000002E-26</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="1"/>
+        <v>2.7609400000000002E-26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4.47794E-23</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="1"/>
+        <v>4.47794E-23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.4836000000000002E-17</v>
+      </c>
+      <c r="C26" s="6">
+        <f>B26*($D$26/6.4836E-17)</f>
+        <v>6.4836000000000002E-17</v>
+      </c>
+      <c r="D26">
+        <f>6.4836E-17</f>
+        <v>6.4836000000000002E-17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.0157699999999998E-21</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C37" si="2">B27*($D$26/6.4836E-17)</f>
+        <v>3.0157699999999998E-21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.6674600000000001E-27</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="2"/>
+        <v>4.6674600000000001E-27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2.0074E-24</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0074E-24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.8817300000000002E-27</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="2"/>
+        <v>2.8817300000000002E-27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="6">
+        <v>5.32606E-32</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="2"/>
+        <v>5.32606E-32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1.15793E-32</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="2"/>
+        <v>1.15793E-32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.3557199999999999E-35</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3557199999999999E-35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="6">
+        <v>2.9209100000000002E-37</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="2"/>
+        <v>2.9209100000000002E-37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="6">
+        <v>5.1875399999999997E-36</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="2"/>
+        <v>5.1875399999999997E-36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1.50413E-33</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="2"/>
+        <v>1.50413E-33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="6">
+        <v>3.7490899999999998E-31</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="2"/>
+        <v>3.7490899999999998E-31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ANV] added shotcrete information to spreadsheet
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B77F45-0573-8F4D-A225-306607ECBF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1613F8B-C198-C64A-A6AC-F6B637A45DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
     <sheet name="U235" sheetId="2" r:id="rId2"/>
     <sheet name="U238" sheetId="3" r:id="rId3"/>
     <sheet name="SE Results" sheetId="4" r:id="rId4"/>
+    <sheet name="Shotcrete Density" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>Decay</t>
   </si>
@@ -177,6 +178,69 @@
   </si>
   <si>
     <t>842110-Po</t>
+  </si>
+  <si>
+    <t>atoms/cm^3</t>
+  </si>
+  <si>
+    <t>overall number density (atoms/cm^3)</t>
+  </si>
+  <si>
+    <t>Z (atomic number)</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Mass Fraction (%)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>overall density (g/cm^3)</t>
+  </si>
+  <si>
+    <t>overall density (kg/m^3)</t>
+  </si>
+  <si>
+    <t>Reference: https://usa.sika.com/dms/getdocument.get/3b1394e4-dd73-4c31-92b6-973d26cb49a5/king-ms-d3.pdf</t>
+  </si>
+  <si>
+    <t>Use MS-D3 shotcrete mentioned in ref: https://confluence.slac.stanford.edu/display/NEXUS/Model+Neutron+Spectrum under "this report"</t>
   </si>
 </sst>
 </file>
@@ -184,7 +248,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -195,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,14 +318,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1994,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2006,9 +2077,11 @@
     <col min="2" max="2" width="24.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2021,8 +2094,14 @@
       <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2037,7 +2116,7 @@
         <v>2.9999999999999998E-14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2050,7 +2129,7 @@
         <v>4.0705599999999999E-24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2063,7 +2142,7 @@
         <v>2.1126800000000001E-26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2075,7 +2154,7 @@
         <v>3.7546900000000003E-30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2087,7 +2166,7 @@
         <v>9.8039200000000002E-33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2099,7 +2178,7 @@
         <v>1.2898000000000001E-38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2112,7 +2191,7 @@
         <v>2.4590199999999999E-28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2125,8 +2204,14 @@
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2141,7 +2226,7 @@
         <v>8.9999999999999995E-15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2154,7 +2239,7 @@
         <v>4.9453300000000002E-19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2167,7 +2252,7 @@
         <v>1.5178200000000001E-19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2180,7 +2265,7 @@
         <v>3.22604E-21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2192,7 +2277,7 @@
         <v>2.1078800000000001E-26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2204,7 +2289,7 @@
         <v>1.9150299999999999E-35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2216,7 +2301,7 @@
         <v>1.1858500000000001E-29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2228,7 +2313,7 @@
         <v>1.04395E-35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2240,7 +2325,7 @@
         <v>7.62767E-25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2337,7 @@
         <v>7.6275999999999997E-29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2264,7 +2349,7 @@
         <v>2.7609400000000002E-26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2276,7 +2361,7 @@
         <v>4.47794E-23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
@@ -2289,8 +2374,14 @@
       <c r="D25" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2306,7 +2397,7 @@
         <v>6.4836000000000002E-17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2318,7 +2409,7 @@
         <v>3.0157699999999998E-21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2330,7 +2421,7 @@
         <v>4.6674600000000001E-27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2342,7 +2433,7 @@
         <v>2.0074E-24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2354,7 +2445,7 @@
         <v>2.8817300000000002E-27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2366,7 +2457,7 @@
         <v>5.32606E-32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2436,6 +2527,187 @@
       <c r="C37" s="6">
         <f t="shared" si="2"/>
         <v>3.7490899999999998E-31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>6.04</v>
+      </c>
+      <c r="D2">
+        <v>2222.2199999999998</v>
+      </c>
+      <c r="E2">
+        <f>D2*(1000)*(1/100000)</f>
+        <v>22.222200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>2.54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="7">
+        <f>SUM(C2:C12)</f>
+        <v>99.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ANV] updated decay chain spreadsheet
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1613F8B-C198-C64A-A6AC-F6B637A45DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D432E-8C5B-BC44-A2C7-D8EFD21FA5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>Decay</t>
   </si>
@@ -72,9 +72,6 @@
     <t>isotopes</t>
   </si>
   <si>
-    <t>overall contamination (ppm)</t>
-  </si>
-  <si>
     <t>902320-Th</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>882240-Ra</t>
   </si>
   <si>
-    <t>232-Th (for 3e-14 ppm)</t>
-  </si>
-  <si>
     <t>scaled</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>832120-Bi</t>
   </si>
   <si>
-    <t>238-U (for 9e-15 ppm)</t>
-  </si>
-  <si>
     <t>922380-U</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>842100-Po</t>
   </si>
   <si>
-    <t>235-U (for 6.4836e-17 ppm)</t>
-  </si>
-  <si>
     <t>922350-U</t>
   </si>
   <si>
@@ -241,6 +229,27 @@
   </si>
   <si>
     <t>Use MS-D3 shotcrete mentioned in ref: https://confluence.slac.stanford.edu/display/NEXUS/Model+Neutron+Spectrum under "this report"</t>
+  </si>
+  <si>
+    <t>Elemental Mass Density (g/cm^3)</t>
+  </si>
+  <si>
+    <t>Molar Mass (amu)</t>
+  </si>
+  <si>
+    <t>Number Density (#/cm^3)</t>
+  </si>
+  <si>
+    <t>overall contamination (per atom)</t>
+  </si>
+  <si>
+    <t>232-Th (for 3e-14 per atom)</t>
+  </si>
+  <si>
+    <t>238-U (for 9e-15 per atom)</t>
+  </si>
+  <si>
+    <t>235-U (for 6.4836e-17 per atom)</t>
   </si>
 </sst>
 </file>
@@ -2067,16 +2076,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
   </cols>
@@ -2086,24 +2095,24 @@
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6">
         <v>2.9999999999999998E-14</v>
@@ -2115,10 +2124,17 @@
       <c r="D2" s="2">
         <v>2.9999999999999998E-14</v>
       </c>
+      <c r="E2" s="6">
+        <f>$F$2*C2</f>
+        <v>19038570000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6">
         <f>4.07056E-24</f>
@@ -2128,10 +2144,14 @@
         <f t="shared" ref="C3:C8" si="0">B3*($D$2/0.00000000000003)</f>
         <v>4.0705599999999999E-24</v>
       </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E9" si="1">$F$2*C3</f>
+        <v>2.5832547166399999</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="6">
         <f>2.11268E-26</f>
@@ -2141,10 +2161,14 @@
         <f t="shared" si="0"/>
         <v>2.1126800000000001E-26</v>
       </c>
+      <c r="E4" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3407468689200001E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6">
         <v>3.7546900000000003E-30</v>
@@ -2153,10 +2177,14 @@
         <f t="shared" si="0"/>
         <v>3.7546900000000003E-30</v>
       </c>
+      <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>2.3827976131100004E-6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6">
         <v>9.8039200000000002E-33</v>
@@ -2165,10 +2193,14 @@
         <f t="shared" si="0"/>
         <v>9.8039200000000002E-33</v>
       </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>6.2217539064800001E-9</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6">
         <v>1.2898000000000001E-38</v>
@@ -2177,10 +2209,14 @@
         <f t="shared" si="0"/>
         <v>1.2898000000000001E-38</v>
       </c>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>8.1853158620000008E-15</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6">
         <f>2.45902E-28</f>
@@ -2190,30 +2226,37 @@
         <f t="shared" si="0"/>
         <v>2.4590199999999999E-28</v>
       </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>1.5605408133800001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6">
         <v>8.9999999999999995E-15</v>
@@ -2225,10 +2268,17 @@
       <c r="D11" s="2">
         <v>8.9999999999999995E-15</v>
       </c>
+      <c r="E11" s="6">
+        <f>$F$11*C11</f>
+        <v>5711571000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6">
         <f>4.94533E-19</f>
@@ -2238,10 +2288,14 @@
         <f>B12/($D$11/0.000000000000009)</f>
         <v>4.9453300000000002E-19</v>
       </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E22" si="2">$F$11*C12</f>
+        <v>313840.03792700003</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6">
         <f>1.51782E-19</f>
@@ -2251,10 +2305,14 @@
         <f>B13/($D$11/0.000000000000009)</f>
         <v>1.5178200000000001E-19</v>
       </c>
+      <c r="E13" s="6">
+        <f t="shared" si="2"/>
+        <v>96323.741058000014</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6">
         <f>3.22604E-21</f>
@@ -2264,101 +2322,137 @@
         <f>B14/($D$11/0.000000000000009)</f>
         <v>3.22604E-21</v>
       </c>
+      <c r="E14" s="6">
+        <f t="shared" si="2"/>
+        <v>2047.3062787599999</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6">
         <v>2.1078800000000001E-26</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" ref="C15:C22" si="1">B15/($D$11/0.000000000000009)</f>
+        <f t="shared" ref="C15:C22" si="3">B15/($D$11/0.000000000000009)</f>
         <v>2.1078800000000001E-26</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3377006977200002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6">
         <v>1.9150299999999999E-35</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9150299999999999E-35</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2153144235699999E-11</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="6">
         <v>1.1858500000000001E-29</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1858500000000001E-29</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="2"/>
+        <v>7.5256294115000006E-6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6">
         <v>1.04395E-35</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.04395E-35</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="2"/>
+        <v>6.6251050504999998E-12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" s="6">
         <v>7.62767E-25</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.62767E-25</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="2"/>
+        <v>0.48406643077299999</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6">
         <v>7.6275999999999997E-29</v>
       </c>
       <c r="C20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6275999999999997E-29</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8406198843999999E-5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6">
         <v>2.7609400000000002E-26</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7609400000000002E-26</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="2"/>
+        <v>1.7521449818600002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" s="6">
         <v>4.47794E-23</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.47794E-23</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="2"/>
+        <v>28.417858048599999</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2366,24 +2460,24 @@
         <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B26" s="6">
         <v>6.4836000000000002E-17</v>
@@ -2396,137 +2490,188 @@
         <f>6.4836E-17</f>
         <v>6.4836000000000002E-17</v>
       </c>
+      <c r="E26" s="6">
+        <f>$F$26*C26</f>
+        <v>41146157.484000005</v>
+      </c>
+      <c r="F26" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B27" s="6">
         <v>3.0157699999999998E-21</v>
       </c>
       <c r="C27" s="6">
-        <f t="shared" ref="C27:C37" si="2">B27*($D$26/6.4836E-17)</f>
+        <f t="shared" ref="C27:C37" si="4">B27*($D$26/6.4836E-17)</f>
         <v>3.0157699999999998E-21</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
+        <v>1913.86494163</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B28" s="6">
         <v>4.6674600000000001E-27</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.6674600000000001E-27</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="5"/>
+        <v>2.96205879774E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B29" s="6">
         <v>2.0074E-24</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.0074E-24</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="5"/>
+        <v>1.2739341806</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B30" s="6">
         <v>2.8817300000000002E-27</v>
       </c>
       <c r="C30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.8817300000000002E-27</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="5"/>
+        <v>1.8288006108700002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B31" s="6">
         <v>5.32606E-32</v>
       </c>
       <c r="C31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.32606E-32</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="5"/>
+        <v>3.3800188711400002E-8</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B32" s="6">
         <v>1.15793E-32</v>
       </c>
       <c r="C32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.15793E-32</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E32" s="6">
+        <f t="shared" si="5"/>
+        <v>7.3484437867000002E-9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33" s="6">
         <v>1.3557199999999999E-35</v>
       </c>
       <c r="C33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3557199999999999E-35</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33" s="6">
+        <f t="shared" si="5"/>
+        <v>8.6036567067999988E-12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B34" s="6">
         <v>2.9209100000000002E-37</v>
       </c>
       <c r="C34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9209100000000002E-37</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E34" s="6">
+        <f t="shared" si="5"/>
+        <v>1.8536649832900002E-13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B35" s="6">
         <v>5.1875399999999997E-36</v>
       </c>
       <c r="C35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.1875399999999997E-36</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E35" s="6">
+        <f t="shared" si="5"/>
+        <v>3.29211144726E-12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B36" s="6">
         <v>1.50413E-33</v>
       </c>
       <c r="C36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.50413E-33</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E36" s="6">
+        <f t="shared" si="5"/>
+        <v>9.5454947647000005E-10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B37" s="6">
         <v>3.7490899999999998E-31</v>
       </c>
       <c r="C37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.7490899999999998E-31</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="5"/>
+        <v>2.3792437467100001E-7</v>
       </c>
     </row>
   </sheetData>
@@ -2536,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2548,28 +2693,40 @@
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -2584,10 +2741,21 @@
         <f>D2*(1000)*(1/100000)</f>
         <v>22.222200000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>$E$2*(C2/100)</f>
+        <v>1.3422208800000002</v>
+      </c>
+      <c r="G2">
+        <v>26.981539000000001</v>
+      </c>
+      <c r="H2">
+        <f>(F2/G2)*6.0221408E+23</f>
+        <v>2.9957680042120296E+22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -2595,13 +2763,21 @@
       <c r="C3">
         <v>9.5399999999999991</v>
       </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">$E$2*(C3/100)</f>
+        <v>2.1199978799999997</v>
+      </c>
+      <c r="G3">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="1">(F3/G3)*6.0221408E+23</f>
+        <v>3.185519668910999E+22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>26</v>
@@ -2609,13 +2785,21 @@
       <c r="C4">
         <v>2.54</v>
       </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.56444388000000001</v>
+      </c>
+      <c r="G4">
+        <v>55.844999999999999</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>6.0867768270360895E+21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>19</v>
@@ -2623,10 +2807,21 @@
       <c r="C5">
         <v>1.76</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.39111072000000002</v>
+      </c>
+      <c r="G5">
+        <v>39.098300000000002</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>6.0241080155131452E+21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -2634,10 +2829,21 @@
       <c r="C6">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.26222195999999998</v>
+      </c>
+      <c r="G6">
+        <v>24.305</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>6.4971716271218591E+21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -2645,10 +2851,21 @@
       <c r="C7">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>8.2222140000000013E-2</v>
+      </c>
+      <c r="G7">
+        <v>54.938043999999998</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>9.0129401759791828E+20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -2656,10 +2873,21 @@
       <c r="C8">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.49999949999999999</v>
+      </c>
+      <c r="G8">
+        <v>22.989768999999999</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.3097423418780763E+22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>14</v>
@@ -2667,10 +2895,21 @@
       <c r="C9">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>6.1999937999999997</v>
+      </c>
+      <c r="G9">
+        <v>28.0855</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.3294132425175638E+23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2678,10 +2917,21 @@
       <c r="C10">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>8.88888E-3</v>
+      </c>
+      <c r="G10">
+        <v>1.0078400000000001</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>5.3113675696840764E+21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -2689,10 +2939,21 @@
       <c r="C11">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>8.88888E-3</v>
+      </c>
+      <c r="G11">
+        <v>12.010999999999999</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>4.4567552172428611E+20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -2700,14 +2961,43 @@
       <c r="C12">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>10.666656</v>
+      </c>
+      <c r="G12">
+        <v>15.999000000000001</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>4.0150074565388331E+23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="7">
         <f>SUM(C2:C12)</f>
         <v>99.66</v>
+      </c>
+      <c r="F13" s="7">
+        <f>SUM(F2:F12)</f>
+        <v>22.146644520000002</v>
+      </c>
+      <c r="H13" s="7">
+        <f>SUM(H2:H12)</f>
+        <v>6.3461876363432809E+23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ANV] updated Th shotcrete contam to 1ppb
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D432E-8C5B-BC44-A2C7-D8EFD21FA5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98DE8CE-DEE5-8543-85AD-4019F69F3EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -2076,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2683,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[ANV] updated shotcrete input files
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98DE8CE-DEE5-8543-85AD-4019F69F3EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B8D738-DCA6-5146-9D18-E2ECDE8666B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -2077,7 +2077,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[ANV] updated the decay chains and stopping element fractions
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B8D738-DCA6-5146-9D18-E2ECDE8666B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319B01D2-BD42-8B4F-8C81-FC2A6BF84FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>Decay</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>235-U (for 6.4836e-17 per atom)</t>
+  </si>
+  <si>
+    <t>fraction of atoms</t>
   </si>
 </sst>
 </file>
@@ -268,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -336,6 +345,7 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2076,7 +2086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2681,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2696,9 +2706,10 @@
     <col min="6" max="6" width="29.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -2723,8 +2734,11 @@
       <c r="H1" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -2752,8 +2766,12 @@
         <f>(F2/G2)*6.0221408E+23</f>
         <v>2.9957680042120296E+22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <f>H2/$H$13</f>
+        <v>4.720578993057023E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2774,8 +2792,12 @@
         <f t="shared" ref="H3:H12" si="1">(F3/G3)*6.0221408E+23</f>
         <v>3.185519668910999E+22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="2">H3/$H$13</f>
+        <v>5.0195800241836508E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -2796,8 +2818,12 @@
         <f t="shared" si="1"/>
         <v>6.0867768270360895E+21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>9.5912336284833428E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2818,8 +2844,12 @@
         <f t="shared" si="1"/>
         <v>6.0241080155131452E+21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>9.492483299759916E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2840,8 +2870,12 @@
         <f t="shared" si="1"/>
         <v>6.4971716271218591E+21</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1.023791290051672E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2862,8 +2896,12 @@
         <f t="shared" si="1"/>
         <v>9.0129401759791828E+20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1.4202133142682343E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -2884,8 +2922,12 @@
         <f t="shared" si="1"/>
         <v>1.3097423418780763E+22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>2.063825428636017E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2906,8 +2948,12 @@
         <f t="shared" si="1"/>
         <v>1.3294132425175638E+23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0.20948218342998465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2928,8 +2974,12 @@
         <f t="shared" si="1"/>
         <v>5.3113675696840764E+21</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>8.3693831226593299E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -2950,8 +3000,12 @@
         <f t="shared" si="1"/>
         <v>4.4567552172428611E+20</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>7.022728404246925E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2972,8 +3026,12 @@
         <f t="shared" si="1"/>
         <v>4.0150074565388331E+23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0.63266447300513629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
@@ -2989,18 +3047,121 @@
         <f>SUM(H2:H12)</f>
         <v>6.3461876363432809E+23</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="7">
+        <f>SUM(I2:I12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
     </row>
+    <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>8.3693831226593299E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>7.022728404246925E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>0.63266447300513629</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>2.063825428636017E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>1.023791290051672E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>4.720578993057023E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>0.20948218342998465</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>9.492483299759916E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>5.0195800241836508E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>1.4202133142682343E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>9.5912336284833428E-3</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:B32">
+    <sortCondition ref="A22:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] updating Th232 input files
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319B01D2-BD42-8B4F-8C81-FC2A6BF84FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EECDD69-AE42-B349-A635-2763F17AF961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2693,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C0C8FF-B22E-AA44-AF26-339606D55407}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[ANV] added files for U decay chains
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EECDD69-AE42-B349-A635-2763F17AF961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0A4FB5-8633-3445-802F-4C6F7805906C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -259,8 +259,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -336,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -345,6 +346,7 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2087,7 +2089,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2272,7 +2274,7 @@
         <v>8.9999999999999995E-15</v>
       </c>
       <c r="C11" s="6">
-        <f>B11/($D$11/0.000000000000009)</f>
+        <f>B11*($D$11/0.000000000000009)</f>
         <v>8.9999999999999995E-15</v>
       </c>
       <c r="D11" s="2">
@@ -2295,11 +2297,11 @@
         <v>4.9453300000000002E-19</v>
       </c>
       <c r="C12" s="6">
-        <f>B12/($D$11/0.000000000000009)</f>
+        <f t="shared" ref="C12:C22" si="2">B12*($D$11/0.000000000000009)</f>
         <v>4.9453300000000002E-19</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" ref="E12:E22" si="2">$F$11*C12</f>
+        <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
         <v>313840.03792700003</v>
       </c>
     </row>
@@ -2312,11 +2314,11 @@
         <v>1.5178200000000001E-19</v>
       </c>
       <c r="C13" s="6">
-        <f>B13/($D$11/0.000000000000009)</f>
+        <f t="shared" si="2"/>
         <v>1.5178200000000001E-19</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96323.741058000014</v>
       </c>
     </row>
@@ -2329,11 +2331,11 @@
         <v>3.22604E-21</v>
       </c>
       <c r="C14" s="6">
-        <f>B14/($D$11/0.000000000000009)</f>
+        <f t="shared" si="2"/>
         <v>3.22604E-21</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2047.3062787599999</v>
       </c>
     </row>
@@ -2345,11 +2347,11 @@
         <v>2.1078800000000001E-26</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" ref="C15:C22" si="3">B15/($D$11/0.000000000000009)</f>
+        <f t="shared" si="2"/>
         <v>2.1078800000000001E-26</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3377006977200002E-2</v>
       </c>
     </row>
@@ -2361,11 +2363,12 @@
         <v>1.9150299999999999E-35</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.9150299999999999E-35</v>
       </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2153144235699999E-11</v>
       </c>
     </row>
@@ -2377,11 +2380,11 @@
         <v>1.1858500000000001E-29</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.1858500000000001E-29</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5256294115000006E-6</v>
       </c>
     </row>
@@ -2393,11 +2396,11 @@
         <v>1.04395E-35</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.04395E-35</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6251050504999998E-12</v>
       </c>
     </row>
@@ -2409,11 +2412,11 @@
         <v>7.62767E-25</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.62767E-25</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.48406643077299999</v>
       </c>
     </row>
@@ -2425,11 +2428,11 @@
         <v>7.6275999999999997E-29</v>
       </c>
       <c r="C20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.6275999999999997E-29</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.8406198843999999E-5</v>
       </c>
     </row>
@@ -2441,11 +2444,11 @@
         <v>2.7609400000000002E-26</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.7609400000000002E-26</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7521449818600002E-2</v>
       </c>
     </row>
@@ -2457,11 +2460,11 @@
         <v>4.47794E-23</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.47794E-23</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28.417858048599999</v>
       </c>
     </row>
@@ -2496,8 +2499,8 @@
         <f>B26*($D$26/6.4836E-17)</f>
         <v>6.4836000000000002E-17</v>
       </c>
-      <c r="D26">
-        <f>6.4836E-17</f>
+      <c r="D26" s="8">
+        <f>0.007204*D11</f>
         <v>6.4836000000000002E-17</v>
       </c>
       <c r="E26" s="6">
@@ -3062,11 +3065,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ANV] updated the decay chains spreadsheet
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0A4FB5-8633-3445-802F-4C6F7805906C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A1344D-978B-F247-A21C-0D319D8687BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
   <si>
     <t>Decay</t>
   </si>
@@ -253,15 +253,28 @@
   </si>
   <si>
     <t>fraction of atoms</t>
+  </si>
+  <si>
+    <t>Q-alpha (MeV)</t>
+  </si>
+  <si>
+    <t>\= doesnt work with SOURCES4C b/c too high alpha energy</t>
+  </si>
+  <si>
+    <t>why?</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -272,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +322,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6360"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -337,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -348,12 +367,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6360"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2086,10 +2116,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2100,9 +2130,11 @@
     <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2121,8 +2153,14 @@
       <c r="F1" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2143,8 +2181,11 @@
       <c r="F2" s="6">
         <v>6.3461900000000002E+23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="11">
+        <v>4.0815999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2160,8 +2201,11 @@
         <f t="shared" ref="E3:E9" si="1">$F$2*C3</f>
         <v>2.5832547166399999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="11">
+        <v>5.5201500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2177,8 +2221,15 @@
         <f t="shared" si="1"/>
         <v>1.3407468689200001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="11">
+        <v>5.7889214999999998</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2193,60 +2244,75 @@
         <f t="shared" si="1"/>
         <v>2.3827976131100004E-6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G5" s="11">
+        <v>6.4047409999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="13">
         <v>9.8039200000000002E-33</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="13">
         <f t="shared" si="0"/>
         <v>9.8039200000000002E-33</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="13">
         <f t="shared" si="1"/>
         <v>6.2217539064800001E-9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="G6" s="14">
+        <v>6.9063499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="13">
         <v>1.2898000000000001E-38</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="13">
         <f t="shared" si="0"/>
         <v>1.2898000000000001E-38</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="13">
         <f t="shared" si="1"/>
         <v>8.1853158620000008E-15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="G7" s="14">
+        <v>8.9541910999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="13">
         <f>2.45902E-28</f>
         <v>2.4590199999999999E-28</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="13">
         <f t="shared" si="0"/>
         <v>2.4590199999999999E-28</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="13">
         <f t="shared" si="1"/>
         <v>1.5605408133800001E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="14">
+        <v>6.2072630000000002</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2265,8 +2331,11 @@
       <c r="F10" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2287,8 +2356,11 @@
       <c r="F11" s="6">
         <v>6.3461900000000002E+23</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="11">
+        <v>4.2699210000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2304,8 +2376,11 @@
         <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
         <v>313840.03792700003</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="11">
+        <v>4.8575699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2321,8 +2396,11 @@
         <f t="shared" si="3"/>
         <v>96323.741058000014</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="11">
+        <v>4.7700149999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2338,8 +2416,11 @@
         <f t="shared" si="3"/>
         <v>2047.3062787599999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="11">
+        <v>4.87073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2354,25 +2435,31 @@
         <f t="shared" si="3"/>
         <v>1.3377006977200002E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="G15" s="11">
+        <v>5.5904299999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="13">
         <v>1.9150299999999999E-35</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="13">
         <f t="shared" si="2"/>
         <v>1.9150299999999999E-35</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="6">
+      <c r="D16" s="15"/>
+      <c r="E16" s="13">
         <f t="shared" si="3"/>
         <v>1.2153144235699999E-11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="14">
+        <v>6.8762999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2387,24 +2474,30 @@
         <f t="shared" si="3"/>
         <v>7.5256294115000006E-6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="G17" s="11">
+        <v>6.1147590000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="13">
         <v>1.04395E-35</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="13">
         <f t="shared" si="2"/>
         <v>1.04395E-35</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="13">
         <f t="shared" si="3"/>
         <v>6.6251050504999998E-12</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="14">
+        <v>7.8335460000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2419,24 +2512,33 @@
         <f t="shared" si="3"/>
         <v>0.48406643077299999</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="G19" s="11">
+        <v>5.4075369999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="13">
         <v>7.6275999999999997E-29</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="13">
         <f t="shared" si="2"/>
         <v>7.6275999999999997E-29</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="13">
         <f t="shared" si="3"/>
         <v>4.8406198843999999E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="14">
+        <v>5.6212999999999997</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2451,8 +2553,11 @@
         <f t="shared" si="3"/>
         <v>1.7521449818600002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="11">
+        <v>5.0365799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2467,8 +2572,11 @@
         <f t="shared" si="3"/>
         <v>28.417858048599999</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="11">
+        <v>3.7921999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
@@ -2487,8 +2595,11 @@
       <c r="F25" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2510,8 +2621,11 @@
       <c r="F26" s="6">
         <v>6.3461900000000002E+23</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="11">
+        <v>4.6781699999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2526,8 +2640,11 @@
         <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
         <v>1913.86494163</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="11">
+        <v>5.1499800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2542,8 +2659,11 @@
         <f t="shared" si="5"/>
         <v>2.96205879774E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="11">
+        <v>6.1466010000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2558,8 +2678,11 @@
         <f t="shared" si="5"/>
         <v>1.2739341806</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="11">
+        <v>5.0422713999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -2574,8 +2697,11 @@
         <f t="shared" si="5"/>
         <v>1.8288006108700002E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="11">
+        <v>5.9789921000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2590,24 +2716,30 @@
         <f t="shared" si="5"/>
         <v>3.3800188711400002E-8</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="G31" s="11">
+        <v>5.5613000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="13">
         <v>1.15793E-32</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="13">
         <f t="shared" si="4"/>
         <v>1.15793E-32</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="13">
         <f t="shared" si="5"/>
         <v>7.3484437867000002E-9</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G32" s="14">
+        <v>6.9462299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2622,69 +2754,84 @@
         <f t="shared" si="5"/>
         <v>8.6036567067999988E-12</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="G33" s="11">
+        <v>6.3425000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="13">
         <v>2.9209100000000002E-37</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="13">
         <f t="shared" si="4"/>
         <v>2.9209100000000002E-37</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="13">
         <f t="shared" si="5"/>
         <v>1.8536649832900002E-13</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="G34" s="14">
+        <v>8.1783999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="13">
         <v>5.1875399999999997E-36</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="13">
         <f t="shared" si="4"/>
         <v>5.1875399999999997E-36</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="13">
         <f t="shared" si="5"/>
         <v>3.29211144726E-12</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="G35" s="14">
+        <v>7.5263799999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="13">
         <v>1.50413E-33</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="13">
         <f t="shared" si="4"/>
         <v>1.50413E-33</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="13">
         <f t="shared" si="5"/>
         <v>9.5454947647000005E-10</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="G36" s="14">
+        <v>7.5946499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="13">
         <v>3.7490899999999998E-31</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="13">
         <f t="shared" si="4"/>
         <v>3.7490899999999998E-31</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="13">
         <f t="shared" si="5"/>
         <v>2.3792437467100001E-7</v>
+      </c>
+      <c r="G37" s="14">
+        <v>6.7504499999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ANV] updated the contamination spreadsheet
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A1344D-978B-F247-A21C-0D319D8687BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4E729-D89A-E84C-AD76-78C9A199F8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Th232" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="U238" sheetId="3" r:id="rId3"/>
     <sheet name="SE Results" sheetId="4" r:id="rId4"/>
     <sheet name="Shotcrete Density" sheetId="5" r:id="rId5"/>
+    <sheet name="1ppb" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="75">
   <si>
     <t>Decay</t>
   </si>
@@ -273,8 +274,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -365,13 +366,13 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -396,9 +397,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -436,7 +437,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -542,7 +543,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -684,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2118,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA64B6C-DEC2-C34F-9D2C-E99132B53E3A}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2199,7 @@
         <v>4.0705599999999999E-24</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E9" si="1">$F$2*C3</f>
+        <f t="shared" ref="E3:E8" si="1">$F$2*C3</f>
         <v>2.5832547166399999</v>
       </c>
       <c r="G3" s="11">
@@ -3314,4 +3315,728 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB4BF7A-0142-9B4A-8871-96C42DF45FD4}">
+  <dimension ref="A1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="C2" s="6">
+        <f>B2*($D$2/0.00000000000003)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E2" s="6">
+        <f>$F$2*C2</f>
+        <v>634619000000000</v>
+      </c>
+      <c r="F2" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G2" s="11">
+        <v>4.0815999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6">
+        <f>4.07056E-24</f>
+        <v>4.0705599999999999E-24</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C8" si="0">B3*($D$2/0.00000000000003)</f>
+        <v>1.3568533333333334E-19</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E8" si="1">$F$2*C3</f>
+        <v>86108.490554666671</v>
+      </c>
+      <c r="G3" s="11">
+        <v>5.5201500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6">
+        <f>2.11268E-26</f>
+        <v>2.1126800000000001E-26</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>7.0422666666666678E-22</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="1"/>
+        <v>446.91562297333343</v>
+      </c>
+      <c r="G4" s="11">
+        <v>5.7889214999999998</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.7546900000000003E-30</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2515633333333336E-25</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>7.9426587103666693E-2</v>
+      </c>
+      <c r="G5" s="11">
+        <v>6.4047409999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="13">
+        <v>9.8039200000000002E-33</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="0"/>
+        <v>3.2679733333333338E-28</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="1"/>
+        <v>2.073917968826667E-4</v>
+      </c>
+      <c r="G6" s="14">
+        <v>6.9063499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1.2898000000000001E-38</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="0"/>
+        <v>4.299333333333334E-34</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="1"/>
+        <v>2.728438620666667E-10</v>
+      </c>
+      <c r="G7" s="14">
+        <v>8.9541910999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13">
+        <f>2.45902E-28</f>
+        <v>2.4590199999999999E-28</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="0"/>
+        <v>8.1967333333333338E-24</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="1"/>
+        <v>5.2018027112666667</v>
+      </c>
+      <c r="G8" s="14">
+        <v>6.2072630000000002</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8.9999999999999995E-15</v>
+      </c>
+      <c r="C11" s="6">
+        <f>B11*($D$11/0.000000000000009)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E11" s="6">
+        <f>$F$11*C11</f>
+        <v>634619000000000</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G11" s="11">
+        <v>4.2699210000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <f>4.94533E-19</f>
+        <v>4.9453300000000002E-19</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:C22" si="2">B12*($D$11/0.000000000000009)</f>
+        <v>5.4948111111111116E-14</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:E22" si="3">$F$11*C12</f>
+        <v>34871115325.222229</v>
+      </c>
+      <c r="G12" s="11">
+        <v>4.8575699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6">
+        <f>1.51782E-19</f>
+        <v>1.5178200000000001E-19</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6864666666666669E-14</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="3"/>
+        <v>10702637895.333336</v>
+      </c>
+      <c r="G13" s="11">
+        <v>4.7700149999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6">
+        <f>3.22604E-21</f>
+        <v>3.22604E-21</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5844888888888891E-16</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="3"/>
+        <v>227478475.41777781</v>
+      </c>
+      <c r="G14" s="11">
+        <v>4.87073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2.1078800000000001E-26</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3420888888888894E-21</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="3"/>
+        <v>1486.3341085777781</v>
+      </c>
+      <c r="G15" s="11">
+        <v>5.5904299999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.9150299999999999E-35</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="2"/>
+        <v>2.1278111111111113E-30</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13">
+        <f t="shared" si="3"/>
+        <v>1.3503493595222223E-6</v>
+      </c>
+      <c r="G16" s="14">
+        <v>6.8762999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.1858500000000001E-29</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3176111111111114E-24</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.8361810457222224</v>
+      </c>
+      <c r="G17" s="11">
+        <v>6.1147590000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1.04395E-35</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="2"/>
+        <v>1.1599444444444446E-30</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="3"/>
+        <v>7.3612278338888901E-7</v>
+      </c>
+      <c r="G18" s="14">
+        <v>7.8335460000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.62767E-25</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="2"/>
+        <v>8.4751888888888893E-20</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="3"/>
+        <v>53785.158974777783</v>
+      </c>
+      <c r="G19" s="11">
+        <v>5.4075369999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="13">
+        <v>7.6275999999999997E-29</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="2"/>
+        <v>8.4751111111111123E-24</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="3"/>
+        <v>5.3784665382222228</v>
+      </c>
+      <c r="G20" s="14">
+        <v>5.6212999999999997</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.7609400000000002E-26</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0677111111111118E-21</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="3"/>
+        <v>1946.8277576222226</v>
+      </c>
+      <c r="G21" s="11">
+        <v>5.0365799999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4.47794E-23</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="2"/>
+        <v>4.9754888888888893E-18</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="3"/>
+        <v>3157539.7831777781</v>
+      </c>
+      <c r="G22" s="11">
+        <v>3.7921999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.4836000000000002E-17</v>
+      </c>
+      <c r="C26" s="6">
+        <f>B26*($D$26/6.4836E-17)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E26" s="6">
+        <f>$F$26*C26</f>
+        <v>634619000000000</v>
+      </c>
+      <c r="F26" s="6">
+        <v>6.3461900000000002E+23</v>
+      </c>
+      <c r="G26" s="11">
+        <v>4.6781699999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6">
+        <v>3.0157699999999998E-21</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C37" si="4">B27*($D$26/6.4836E-17)</f>
+        <v>4.6513819483003271E-14</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" ref="E27:E37" si="5">$F$26*C27</f>
+        <v>29518553606.484055</v>
+      </c>
+      <c r="G27" s="11">
+        <v>5.1499800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.6674600000000001E-27</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1988709975939301E-20</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="5"/>
+        <v>45685.403136220622</v>
+      </c>
+      <c r="G28" s="11">
+        <v>6.1466010000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2.0074E-24</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="4"/>
+        <v>3.0961194398173858E-17</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="5"/>
+        <v>19648562.227774695</v>
+      </c>
+      <c r="G29" s="11">
+        <v>5.0422713999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.8817300000000002E-27</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="4"/>
+        <v>4.4446449503362333E-20</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="5"/>
+        <v>28206.5613373743</v>
+      </c>
+      <c r="G30" s="11">
+        <v>5.9789921000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6">
+        <v>5.32606E-32</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="4"/>
+        <v>8.2146646924548096E-25</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="5"/>
+        <v>0.52131822924609794</v>
+      </c>
+      <c r="G31" s="11">
+        <v>5.5613000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1.15793E-32</v>
+      </c>
+      <c r="C32" s="13">
+        <f t="shared" si="4"/>
+        <v>1.7859368252205565E-25</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="5"/>
+        <v>0.11333894420846444</v>
+      </c>
+      <c r="G32" s="14">
+        <v>6.9462299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1.3557199999999999E-35</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="4"/>
+        <v>2.0909988278117094E-28</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="5"/>
+        <v>1.3269875851070392E-4</v>
+      </c>
+      <c r="G33" s="11">
+        <v>6.3425000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2.9209100000000002E-37</v>
+      </c>
+      <c r="C34" s="13">
+        <f t="shared" si="4"/>
+        <v>4.5050743414152638E-30</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="5"/>
+        <v>2.8590057734746135E-6</v>
+      </c>
+      <c r="G34" s="14">
+        <v>8.1783999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5.1875399999999997E-36</v>
+      </c>
+      <c r="C35" s="13">
+        <f t="shared" si="4"/>
+        <v>8.0010179529890804E-29</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0775980123079771E-5</v>
+      </c>
+      <c r="G35" s="14">
+        <v>7.5263799999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1.50413E-33</v>
+      </c>
+      <c r="C36" s="13">
+        <f t="shared" si="4"/>
+        <v>2.3198994385835032E-26</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="5"/>
+        <v>1.4722522618144242E-2</v>
+      </c>
+      <c r="G36" s="14">
+        <v>7.5946499999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="13">
+        <v>3.7490899999999998E-31</v>
+      </c>
+      <c r="C37" s="13">
+        <f t="shared" si="4"/>
+        <v>5.782420260349189E-24</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="5"/>
+        <v>3.6696337632025422</v>
+      </c>
+      <c r="G37" s="14">
+        <v>6.7504499999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] updated a figure
</commit_message>
<xml_diff>
--- a/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
+++ b/neutron-bknd-spectra/decay_chains/decay_chains_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/L3He_paper2023/neutron-bknd-spectra/decay_chains/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4E729-D89A-E84C-AD76-78C9A199F8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEA7164-FC05-EA49-ADFE-2DCDBE14B1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -2120,7 +2120,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2845,7 +2845,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3322,7 +3322,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3378,7 +3378,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="E2" s="6">
-        <f>$F$2*C2</f>
+        <f t="shared" ref="E2:E8" si="0">$F$2*C2</f>
         <v>634619000000000</v>
       </c>
       <c r="F2" s="6">
@@ -3397,11 +3397,11 @@
         <v>4.0705599999999999E-24</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C8" si="0">B3*($D$2/0.00000000000003)</f>
+        <f t="shared" ref="C3:C8" si="1">B3*($D$2/0.00000000000003)</f>
         <v>1.3568533333333334E-19</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E8" si="1">$F$2*C3</f>
+        <f t="shared" si="0"/>
         <v>86108.490554666671</v>
       </c>
       <c r="G3" s="11">
@@ -3417,11 +3417,11 @@
         <v>2.1126800000000001E-26</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0422666666666678E-22</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>446.91562297333343</v>
       </c>
       <c r="G4" s="11">
@@ -3440,11 +3440,11 @@
         <v>3.7546900000000003E-30</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2515633333333336E-25</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.9426587103666693E-2</v>
       </c>
       <c r="G5" s="11">
@@ -3459,11 +3459,11 @@
         <v>9.8039200000000002E-33</v>
       </c>
       <c r="C6" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2679733333333338E-28</v>
       </c>
       <c r="E6" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.073917968826667E-4</v>
       </c>
       <c r="G6" s="14">
@@ -3478,11 +3478,11 @@
         <v>1.2898000000000001E-38</v>
       </c>
       <c r="C7" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.299333333333334E-34</v>
       </c>
       <c r="E7" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.728438620666667E-10</v>
       </c>
       <c r="G7" s="14">
@@ -3498,11 +3498,11 @@
         <v>2.4590199999999999E-28</v>
       </c>
       <c r="C8" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.1967333333333338E-24</v>
       </c>
       <c r="E8" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.2018027112666667</v>
       </c>
       <c r="G8" s="14">

</xml_diff>